<commit_message>
Change tabs to spaces
</commit_message>
<xml_diff>
--- a/src/spreadsheets/aws.xlsx
+++ b/src/spreadsheets/aws.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\developers-cheat-sheet\src\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39F9BD95-3981-457D-A16E-6BF8895EA380}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D39ABF-CF21-4A11-A4B6-4985ADE2506D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{AC50BE90-470E-4ADB-ABB4-54CE8C3071A4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Java" sheetId="1" r:id="rId1"/>
+    <sheet name="AWS" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,25 +41,6 @@
     <t>Command(s)</t>
   </si>
   <si>
-    <t>exports.handler = async (event, context, callback) =&gt; {
- const hasError = event['queryStringParameters']['myErrorParam'];
- if (hasError === 'yes') {
-  callback(new Error('My error message'));
-    }
- else {
-  const response = {
-   statusCode: 200,
-   headers: {"Access-Control-Allow-Origin": "*"},
-   body: JSON.stringify({success: true}),
-   isBase64Encoded: false
-  }
-  callback(null, response);
-}</t>
-  </si>
-  <si>
-    <t>Starter Lambda function compatible with API Gateway</t>
-  </si>
-  <si>
     <t>:: This batch file redeploys an existing lambda function
 :: Usage: deploy-existing.bat getAllProducts
 echo off
@@ -74,6 +55,25 @@
   </si>
   <si>
     <t>Batch script to update an existing Lambda function that uses a Lambda Layer. Assumes local layer name is ./helpers and layer on AWS Lambda is located at /opt/lambdas/helpers</t>
+  </si>
+  <si>
+    <t>exports.handler = async (event, context, callback) =&gt; {
+    const hasError = event['queryStringParameters']['myErrorParam'];
+    if (hasError === 'yes') {
+        callback(new Error('My error message'));
+    }
+    else {
+        const response = {
+            statusCode: 200,
+            headers: {"Access-Control-Allow-Origin": "*"},
+            body: JSON.stringify({success: true}),
+            isBase64Encoded: false
+        };
+        callback(null, response);
+}</t>
+  </si>
+  <si>
+    <t>Starter Lambda function compatible with API Gateway v1.0</t>
   </si>
 </sst>
 </file>
@@ -439,8 +439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A1EDD08-339E-4F53-A8CC-87B11A1193DB}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -459,18 +459,18 @@
     </row>
     <row r="2" spans="1:2" ht="203" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="174" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="174" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Add a code block feature
</commit_message>
<xml_diff>
--- a/src/spreadsheets/aws.xlsx
+++ b/src/spreadsheets/aws.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\developers-cheat-sheet\src\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D39ABF-CF21-4A11-A4B6-4985ADE2506D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B5077C-07F6-499E-AFAF-FB84F8D900A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{AC50BE90-470E-4ADB-ABB4-54CE8C3071A4}"/>
   </bookViews>
@@ -41,23 +41,14 @@
     <t>Command(s)</t>
   </si>
   <si>
-    <t>:: This batch file redeploys an existing lambda function
-:: Usage: deploy-existing.bat getAllProducts
-echo off
-echo WARNING: this will delete any index.js or index.zip you have in the current directory!
-pause
-set /p toDeploy=Enter lambda name (without the .js): 
-powershell -Command "(gc %toDeploy%.js) -replace './helpers', '/opt/lambdas/helpers' | Out-File -encoding ASCII index.js"
-powershell "Compress-Archive index.js index.zip"
-aws lambda update-function-code --function-name %toDeploy% --zip-file fileb://index.zip
-del index.js
-del index.zip</t>
-  </si>
-  <si>
     <t>Batch script to update an existing Lambda function that uses a Lambda Layer. Assumes local layer name is ./helpers and layer on AWS Lambda is located at /opt/lambdas/helpers</t>
   </si>
   <si>
-    <t>exports.handler = async (event, context, callback) =&gt; {
+    <t>Starter Lambda function compatible with API Gateway v1.0</t>
+  </si>
+  <si>
+    <t>(CODEBLOCK)
+exports.handler = async (event, context, callback) =&gt; {
     const hasError = event['queryStringParameters']['myErrorParam'];
     if (hasError === 'yes') {
         callback(new Error('My error message'));
@@ -73,7 +64,18 @@
 }</t>
   </si>
   <si>
-    <t>Starter Lambda function compatible with API Gateway v1.0</t>
+    <t>(CODEBLOCK)
+:: This batch file redeploys an existing lambda function
+:: Usage: deploy-existing.bat getAllProducts
+echo off
+echo WARNING: this will delete any index.js or index.zip you have in the current directory!
+pause
+set /p toDeploy=Enter lambda name (without the .js): 
+powershell -Command "(gc %toDeploy%.js) -replace './helpers', '/opt/lambdas/helpers' | Out-File -encoding ASCII index.js"
+powershell "Compress-Archive index.js index.zip"
+aws lambda update-function-code --function-name %toDeploy% --zip-file fileb://index.zip
+del index.js
+del index.zip</t>
   </si>
 </sst>
 </file>
@@ -439,8 +441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A1EDD08-339E-4F53-A8CC-87B11A1193DB}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -457,20 +459,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="203" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="174" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>